<commit_message>
Changed PB1 to PA8 * my PB1 is cooked :(
</commit_message>
<xml_diff>
--- a/doc/WeAct STM32H750 Pinout.xlsx
+++ b/doc/WeAct STM32H750 Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\stm32h750-z80emu\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F1DEAD-CBDD-46B7-B18E-173A93F92368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D801A731-72F7-4002-986D-2962101224AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FD682878-73C0-47F4-AE46-EEDB4B1498C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{FD682878-73C0-47F4-AE46-EEDB4B1498C7}"/>
   </bookViews>
   <sheets>
     <sheet name="stm32h750vbt6 (top)" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="131">
   <si>
     <t>PE1</t>
   </si>
@@ -526,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -590,6 +590,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,8 +937,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,10 +1202,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26" t="s">
         <v>68</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1204,10 +1212,10 @@
       <c r="D15" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="27" t="s">
         <v>35</v>
       </c>
       <c r="H15" s="5" t="s">
@@ -1383,10 +1391,13 @@
   <dimension ref="A2:U14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="21" width="5.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1824,6 +1835,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1832,8 +1844,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,11 +2104,11 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
-        <v>86</v>
+      <c r="D15" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>107</v>
@@ -2104,12 +2116,10 @@
       <c r="G15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>101</v>
-      </c>
+      <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">

</xml_diff>